<commit_message>
update the system modules
brand | manufacture
</commit_message>
<xml_diff>
--- a/douments/ER Support Doument.xlsx
+++ b/douments/ER Support Doument.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\bit\douments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6EF378-EDF2-4533-9648-5AC22181A04A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0709D17F-9D6B-440E-AF7B-E683C211E700}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25416" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -204,9 +204,6 @@
     <t>MSI</t>
   </si>
   <si>
-    <t>manifacture</t>
-  </si>
-  <si>
     <t>manifacture_name</t>
   </si>
   <si>
@@ -397,6 +394,9 @@
   </si>
   <si>
     <t>faq_id</t>
+  </si>
+  <si>
+    <t>manufacturers</t>
   </si>
 </sst>
 </file>
@@ -755,8 +755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1088,7 +1088,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
         <v>53</v>
@@ -1112,7 +1112,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F27" t="s">
         <v>57</v>
@@ -1125,295 +1125,295 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>123</v>
+      </c>
+      <c r="B30" t="s">
         <v>59</v>
       </c>
-      <c r="B30" t="s">
-        <v>60</v>
-      </c>
       <c r="F30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F34" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" t="s">
         <v>94</v>
-      </c>
-      <c r="B39" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B49" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>71</v>
+      </c>
+      <c r="B52" t="s">
         <v>72</v>
-      </c>
-      <c r="B52" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B65" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>110</v>
+      </c>
+      <c r="B68" t="s">
         <v>111</v>
-      </c>
-      <c r="B68" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B72" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" t="s">
         <v>82</v>
-      </c>
-      <c r="B80" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
+        <v>116</v>
+      </c>
+      <c r="B85" t="s">
         <v>117</v>
-      </c>
-      <c r="B85" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
+        <v>121</v>
+      </c>
+      <c r="B90" t="s">
         <v>122</v>
-      </c>
-      <c r="B90" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>